<commit_message>
Update excel data with random puzzle data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicag/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E80271D3-A591-C942-A4E7-EB8B08846343}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AE8247-E773-A848-9062-B43CB502FA2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14580" xr2:uid="{5A0C402A-18EF-2249-A35F-8B40CB33FF1B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>Uniform Cost</t>
   </si>
@@ -1293,6 +1293,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3790714547624925E-3"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1821,6 +1829,959 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Nodes Expanded</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$75</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$74:$F$74</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Uniform Cost</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Misplaced Tile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manhattan Distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$75:$F$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8917</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-12B3-5448-878A-DC0ED2951BB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$76</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$74:$F$74</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Uniform Cost</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Misplaced Tile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manhattan Distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$76:$F$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>17676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-12B3-5448-878A-DC0ED2951BB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$77</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$74:$F$74</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Uniform Cost</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Misplaced Tile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manhattan Distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$77:$F$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>122055</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>891</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-12B3-5448-878A-DC0ED2951BB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1693279839"/>
+        <c:axId val="1610111535"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1693279839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1610111535"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1610111535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1693279839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Max</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Queue Size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$89</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$88:$F$88</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Uniform Cost</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Misplaced Tile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manhattan Distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$89:$F$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C885-6241-A792-CF3915FF448E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$88:$F$88</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Uniform Cost</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Misplaced Tile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manhattan Distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$90:$F$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9457</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>553</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C885-6241-A792-CF3915FF448E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$91</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$D$88:$F$88</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Uniform Cost</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Misplaced Tile</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Manhattan Distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$91:$F$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>46295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4310</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>543</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C885-6241-A792-CF3915FF448E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1691146575"/>
+        <c:axId val="1686594575"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1691146575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1686594575"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1686594575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1691146575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1941,6 +2902,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3470,6 +4511,1012 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3565,16 +5612,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>577853</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>196547</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>305710</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>166310</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>136073</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>112631</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>15119</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>30238</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3596,6 +5643,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>75596</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>166310</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>483811</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>102688</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A93814B6-9CD4-CD4F-83B5-AE1CD1C21EC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>680357</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>120951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>801311</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>45114</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34EF209F-18C8-524F-9AFE-8790003AE7FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3901,18 +6020,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9A50D3-40CA-3F45-86C7-19E4C4AD0426}">
-  <dimension ref="B2:E52"/>
+  <dimension ref="B2:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="84" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="84" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
@@ -4171,6 +6291,122 @@
       </c>
       <c r="E52">
         <v>0.17155000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>8917</v>
+      </c>
+      <c r="E75">
+        <v>608</v>
+      </c>
+      <c r="F75">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>17676</v>
+      </c>
+      <c r="E76">
+        <v>796</v>
+      </c>
+      <c r="F76">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>122055</v>
+      </c>
+      <c r="E77">
+        <v>6931</v>
+      </c>
+      <c r="F77">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>1</v>
+      </c>
+      <c r="F88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>5903</v>
+      </c>
+      <c r="E89">
+        <v>379</v>
+      </c>
+      <c r="F89">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90">
+        <v>9457</v>
+      </c>
+      <c r="E90">
+        <v>553</v>
+      </c>
+      <c r="F90">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <v>46295</v>
+      </c>
+      <c r="E91">
+        <v>4310</v>
+      </c>
+      <c r="F91">
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>